<commit_message>
change between different item options
</commit_message>
<xml_diff>
--- a/ItemDataBase.xlsx
+++ b/ItemDataBase.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS\Documentos\PROYECTOS\Arena\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS\Documentos\PROYECTOS\GladiatorMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="0" windowWidth="27690" windowHeight="12795" xr2:uid="{FD9C3489-AB8B-42CA-8AEA-AA90E3DC7812}"/>
+    <workbookView xWindow="2220" yWindow="0" windowWidth="27690" windowHeight="12795" xr2:uid="{FD9C3489-AB8B-42CA-8AEA-AA90E3DC7812}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,23 +25,23 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{72981864-0E5D-4006-A014-FC243E3C94F4}" name="ItemDataBase" type="4" refreshedVersion="0" background="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="ItemDataBase" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Doctor Holmes\Desktop\ItemDataBase.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" xr16:uid="{F79E9071-661F-4D90-A855-96EB77837663}" name="ItemDataBase1" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="ItemDataBase1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Doctor Holmes\Desktop\ItemDataBase.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" xr16:uid="{10967524-1A29-4DEB-85F8-C60364F50F0F}" name="ItemDataBase2" type="4" refreshedVersion="0" background="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="ItemDataBase2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Doctor Holmes\Desktop\ItemDataBase.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="4" xr16:uid="{58939BD8-30A6-4115-A30F-573C450A41FC}" name="ItemDataBase3" type="4" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="ItemDataBase3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Doctor Holmes\Desktop\ItemDataBase.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="118">
   <si>
     <t>Name</t>
   </si>
@@ -341,6 +341,60 @@
   </si>
   <si>
     <t>Torso 2</t>
+  </si>
+  <si>
+    <t>Right Leg 1</t>
+  </si>
+  <si>
+    <t>Right Leg 3</t>
+  </si>
+  <si>
+    <t>Right Leg 2</t>
+  </si>
+  <si>
+    <t>leg_1_r</t>
+  </si>
+  <si>
+    <t>leg_2_r</t>
+  </si>
+  <si>
+    <t>leg_3_r</t>
+  </si>
+  <si>
+    <t>R_Leg_1</t>
+  </si>
+  <si>
+    <t>R_Leg_2</t>
+  </si>
+  <si>
+    <t>R_Leg_3</t>
+  </si>
+  <si>
+    <t>Left Leg 2</t>
+  </si>
+  <si>
+    <t>Left Leg 3</t>
+  </si>
+  <si>
+    <t>Left Leg 1</t>
+  </si>
+  <si>
+    <t>leg_1_l</t>
+  </si>
+  <si>
+    <t>leg_2_l</t>
+  </si>
+  <si>
+    <t>leg_3_l</t>
+  </si>
+  <si>
+    <t>L_Leg_1</t>
+  </si>
+  <si>
+    <t>L_Leg_2</t>
+  </si>
+  <si>
+    <t>L_Leg_3</t>
   </si>
 </sst>
 </file>
@@ -454,8 +508,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{5BA81B61-FF4B-4070-AFDD-483010E0F5E2}" name="Table18" displayName="Table18" ref="B5:F41" tableType="xml" totalsRowShown="0" connectionId="4">
-  <autoFilter ref="B5:F41" xr:uid="{9C5E23C4-2A17-4A45-9E0D-FA782667747E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{5BA81B61-FF4B-4070-AFDD-483010E0F5E2}" name="Table18" displayName="Table18" ref="B5:F47" tableType="xml" totalsRowShown="0" connectionId="4">
+  <autoFilter ref="B5:F47" xr:uid="{9C5E23C4-2A17-4A45-9E0D-FA782667747E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{20C3BA91-A104-45DF-8336-8663BB83979E}" uniqueName="Name" name="Name">
       <xmlColumnPr mapId="4" xpath="/ItemDataBase/Item/Name" xmlDataType="string"/>
@@ -774,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D766CA4A-594E-4340-8F54-93E0D16A5559}">
-  <dimension ref="A5:U41"/>
+  <dimension ref="A5:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,7 +1054,9 @@
       <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
       <c r="D20" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1071,9 @@
       <c r="B21" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
       <c r="D21" t="s">
         <v>34</v>
       </c>
@@ -1035,7 +1093,9 @@
       <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
       <c r="D22" t="s">
         <v>35</v>
       </c>
@@ -1050,7 +1110,9 @@
       <c r="B23" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
       <c r="D23" t="s">
         <v>36</v>
       </c>
@@ -1065,7 +1127,9 @@
       <c r="B24" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
       <c r="D24" t="s">
         <v>37</v>
       </c>
@@ -1080,12 +1144,14 @@
       <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
       <c r="D25" t="s">
         <v>38</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
         <v>83</v>
@@ -1095,12 +1161,14 @@
       <c r="B26" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
       <c r="D26" t="s">
         <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
         <v>84</v>
@@ -1110,7 +1178,9 @@
       <c r="B27" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
       <c r="D27" t="s">
         <v>40</v>
       </c>
@@ -1125,7 +1195,9 @@
       <c r="B28" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
       <c r="D28" t="s">
         <v>41</v>
       </c>
@@ -1140,7 +1212,9 @@
       <c r="B29" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
       <c r="D29" t="s">
         <v>42</v>
       </c>
@@ -1155,7 +1229,9 @@
       <c r="B30" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
       <c r="D30" t="s">
         <v>43</v>
       </c>
@@ -1170,7 +1246,9 @@
       <c r="B31" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
       <c r="D31" t="s">
         <v>44</v>
       </c>
@@ -1185,12 +1263,14 @@
       <c r="B32" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
       <c r="D32" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s">
         <v>81</v>
@@ -1200,12 +1280,14 @@
       <c r="B33" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="1"/>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
       <c r="D33" t="s">
         <v>46</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F33" t="s">
         <v>79</v>
@@ -1215,7 +1297,9 @@
       <c r="B34" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
       <c r="D34" t="s">
         <v>47</v>
       </c>
@@ -1230,7 +1314,9 @@
       <c r="B35" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
       <c r="D35" t="s">
         <v>48</v>
       </c>
@@ -1245,7 +1331,9 @@
       <c r="B36" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
       <c r="D36" t="s">
         <v>49</v>
       </c>
@@ -1260,7 +1348,9 @@
       <c r="B37" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" t="s">
+        <v>62</v>
+      </c>
       <c r="D37" t="s">
         <v>50</v>
       </c>
@@ -1275,7 +1365,9 @@
       <c r="B38" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="1"/>
+      <c r="C38" t="s">
+        <v>57</v>
+      </c>
       <c r="D38" t="s">
         <v>51</v>
       </c>
@@ -1290,7 +1382,9 @@
       <c r="B39" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="1"/>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
       <c r="D39" t="s">
         <v>52</v>
       </c>
@@ -1305,7 +1399,9 @@
       <c r="B40" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="1"/>
+      <c r="C40" t="s">
+        <v>97</v>
+      </c>
       <c r="D40" t="s">
         <v>93</v>
       </c>
@@ -1323,7 +1419,9 @@
       <c r="B41" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="1"/>
+      <c r="C41" t="s">
+        <v>99</v>
+      </c>
       <c r="D41" t="s">
         <v>94</v>
       </c>
@@ -1332,6 +1430,108 @@
       </c>
       <c r="F41" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" t="s">
+        <v>104</v>
+      </c>
+      <c r="E43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" t="s">
+        <v>114</v>
+      </c>
+      <c r="E47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some 3d models changed
</commit_message>
<xml_diff>
--- a/ItemDataBase.xlsx
+++ b/ItemDataBase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="0" windowWidth="27690" windowHeight="12795" xr2:uid="{FD9C3489-AB8B-42CA-8AEA-AA90E3DC7812}"/>
+    <workbookView xWindow="5550" yWindow="0" windowWidth="27690" windowHeight="12795" xr2:uid="{FD9C3489-AB8B-42CA-8AEA-AA90E3DC7812}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -127,280 +127,262 @@
     <t>shoulder_2_r</t>
   </si>
   <si>
+    <t>arm_1_l</t>
+  </si>
+  <si>
+    <t>arm_2_l</t>
+  </si>
+  <si>
+    <t>arm_3_l</t>
+  </si>
+  <si>
+    <t>shoulder_1_l</t>
+  </si>
+  <si>
+    <t>shoulder_2_l</t>
+  </si>
+  <si>
+    <t>Helmet 1</t>
+  </si>
+  <si>
+    <t>Helmet 2</t>
+  </si>
+  <si>
+    <t>Helmet 3</t>
+  </si>
+  <si>
+    <t>Helmet 4</t>
+  </si>
+  <si>
+    <t>Shoulder Armour 1 L</t>
+  </si>
+  <si>
+    <t>Shoulder Armour 2 L</t>
+  </si>
+  <si>
+    <t>Arm Armour 3 L</t>
+  </si>
+  <si>
+    <t>Arm Armour 1 L</t>
+  </si>
+  <si>
+    <t>Arm Armour 2 L</t>
+  </si>
+  <si>
+    <t>Shoulder Armour 2 R</t>
+  </si>
+  <si>
+    <t>Shoulder Armour 1 R</t>
+  </si>
+  <si>
+    <t>Arm Armour 3 R</t>
+  </si>
+  <si>
+    <t>Arm Armour 2 R</t>
+  </si>
+  <si>
+    <t>Arm Armour 1 R</t>
+  </si>
+  <si>
+    <t>L_Shoulder_1</t>
+  </si>
+  <si>
+    <t>L_Shoulder_2</t>
+  </si>
+  <si>
+    <t>L_Arm_3</t>
+  </si>
+  <si>
+    <t>L_Arm_1</t>
+  </si>
+  <si>
+    <t>L_Arm_2</t>
+  </si>
+  <si>
+    <t>R_Arm_1</t>
+  </si>
+  <si>
+    <t>R_Arm_2</t>
+  </si>
+  <si>
+    <t>R_Arm_3</t>
+  </si>
+  <si>
+    <t>R_Shoulder_1</t>
+  </si>
+  <si>
+    <t>R_Shoulder_2</t>
+  </si>
+  <si>
+    <t>Helmet_1</t>
+  </si>
+  <si>
+    <t>Helmet_2</t>
+  </si>
+  <si>
+    <t>Helmet_3</t>
+  </si>
+  <si>
+    <t>Helmet_4</t>
+  </si>
+  <si>
+    <t>torso_1</t>
+  </si>
+  <si>
+    <t>torso_2</t>
+  </si>
+  <si>
+    <t>Torso_1</t>
+  </si>
+  <si>
+    <t>Torso_2</t>
+  </si>
+  <si>
+    <t>Torso 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Torso 2</t>
+  </si>
+  <si>
+    <t>Right Leg 1</t>
+  </si>
+  <si>
+    <t>Right Leg 3</t>
+  </si>
+  <si>
+    <t>Right Leg 2</t>
+  </si>
+  <si>
+    <t>leg_1_r</t>
+  </si>
+  <si>
+    <t>leg_2_r</t>
+  </si>
+  <si>
+    <t>leg_3_r</t>
+  </si>
+  <si>
+    <t>R_Leg_1</t>
+  </si>
+  <si>
+    <t>R_Leg_2</t>
+  </si>
+  <si>
+    <t>R_Leg_3</t>
+  </si>
+  <si>
+    <t>Left Leg 2</t>
+  </si>
+  <si>
+    <t>Left Leg 3</t>
+  </si>
+  <si>
+    <t>Left Leg 1</t>
+  </si>
+  <si>
+    <t>leg_1_l</t>
+  </si>
+  <si>
+    <t>leg_2_l</t>
+  </si>
+  <si>
+    <t>leg_3_l</t>
+  </si>
+  <si>
+    <t>L_Leg_1</t>
+  </si>
+  <si>
+    <t>L_Leg_2</t>
+  </si>
+  <si>
+    <t>L_Leg_3</t>
+  </si>
+  <si>
+    <t>Shield 1</t>
+  </si>
+  <si>
+    <t>Shield 2</t>
+  </si>
+  <si>
+    <t>Shield 3</t>
+  </si>
+  <si>
+    <t>shield_1</t>
+  </si>
+  <si>
+    <t>shield_2</t>
+  </si>
+  <si>
+    <t>shield_3</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Shield_1</t>
+  </si>
+  <si>
+    <t>Shield_2</t>
+  </si>
+  <si>
+    <t>Shield_3</t>
+  </si>
+  <si>
+    <t>weapon_1_r</t>
+  </si>
+  <si>
+    <t>weapon_2_r</t>
+  </si>
+  <si>
+    <t>weapon_1_l</t>
+  </si>
+  <si>
+    <t>weapon_2_l</t>
+  </si>
+  <si>
+    <t>R_Gladius_1</t>
+  </si>
+  <si>
+    <t>L_Gladius_1</t>
+  </si>
+  <si>
+    <t>R_Pugio_1</t>
+  </si>
+  <si>
+    <t>L_Pugio_1</t>
+  </si>
+  <si>
+    <t>Right Gladius 1</t>
+  </si>
+  <si>
+    <t>Left Gladius 1</t>
+  </si>
+  <si>
+    <t>Right Pugio 1</t>
+  </si>
+  <si>
+    <t>Left Pugio 1</t>
+  </si>
+  <si>
+    <t>Shoulder Armour 3 L</t>
+  </si>
+  <si>
+    <t>shoulder_3_l</t>
+  </si>
+  <si>
+    <t>L_Shoulder_3</t>
+  </si>
+  <si>
+    <t>Shoulder Armour 3 R</t>
+  </si>
+  <si>
     <t>shoulder_3_r</t>
   </si>
   <si>
-    <t>shoulder_4_r</t>
-  </si>
-  <si>
-    <t>arm_1_l</t>
-  </si>
-  <si>
-    <t>arm_2_l</t>
-  </si>
-  <si>
-    <t>arm_3_l</t>
-  </si>
-  <si>
-    <t>shoulder_1_l</t>
-  </si>
-  <si>
-    <t>shoulder_2_l</t>
-  </si>
-  <si>
-    <t>shoulder_3_l</t>
-  </si>
-  <si>
-    <t>shoulder_4_l</t>
-  </si>
-  <si>
-    <t>Helmet 1</t>
-  </si>
-  <si>
-    <t>Helmet 2</t>
-  </si>
-  <si>
-    <t>Helmet 3</t>
-  </si>
-  <si>
-    <t>Helmet 4</t>
-  </si>
-  <si>
-    <t>Shoulder Armour 1 L</t>
-  </si>
-  <si>
-    <t>Shoulder Armour 2 L</t>
-  </si>
-  <si>
-    <t>Shoulder Armour 3 L</t>
-  </si>
-  <si>
-    <t>Shoulder Armour 4 L</t>
-  </si>
-  <si>
-    <t>Arm Armour 3 L</t>
-  </si>
-  <si>
-    <t>Arm Armour 1 L</t>
-  </si>
-  <si>
-    <t>Arm Armour 2 L</t>
-  </si>
-  <si>
-    <t>Shoulder Armour 4 R</t>
-  </si>
-  <si>
-    <t>Shoulder Armour 3 R</t>
-  </si>
-  <si>
-    <t>Shoulder Armour 2 R</t>
-  </si>
-  <si>
-    <t>Shoulder Armour 1 R</t>
-  </si>
-  <si>
-    <t>Arm Armour 3 R</t>
-  </si>
-  <si>
-    <t>Arm Armour 2 R</t>
-  </si>
-  <si>
-    <t>Arm Armour 1 R</t>
-  </si>
-  <si>
-    <t>L_Shoulder_4</t>
-  </si>
-  <si>
-    <t>L_Shoulder_1</t>
-  </si>
-  <si>
-    <t>L_Shoulder_2</t>
-  </si>
-  <si>
-    <t>L_Shoulder_3</t>
-  </si>
-  <si>
-    <t>L_Arm_3</t>
-  </si>
-  <si>
-    <t>L_Arm_1</t>
-  </si>
-  <si>
-    <t>L_Arm_2</t>
-  </si>
-  <si>
-    <t>R_Arm_1</t>
-  </si>
-  <si>
-    <t>R_Arm_2</t>
-  </si>
-  <si>
-    <t>R_Arm_3</t>
-  </si>
-  <si>
-    <t>R_Shoulder_1</t>
-  </si>
-  <si>
-    <t>R_Shoulder_2</t>
-  </si>
-  <si>
     <t>R_Shoulder_3</t>
-  </si>
-  <si>
-    <t>R_Shoulder_4</t>
-  </si>
-  <si>
-    <t>Helmet_1</t>
-  </si>
-  <si>
-    <t>Helmet_2</t>
-  </si>
-  <si>
-    <t>Helmet_3</t>
-  </si>
-  <si>
-    <t>Helmet_4</t>
-  </si>
-  <si>
-    <t>torso_1</t>
-  </si>
-  <si>
-    <t>torso_2</t>
-  </si>
-  <si>
-    <t>Torso_1</t>
-  </si>
-  <si>
-    <t>Torso_2</t>
-  </si>
-  <si>
-    <t>Torso 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Torso 2</t>
-  </si>
-  <si>
-    <t>Right Leg 1</t>
-  </si>
-  <si>
-    <t>Right Leg 3</t>
-  </si>
-  <si>
-    <t>Right Leg 2</t>
-  </si>
-  <si>
-    <t>leg_1_r</t>
-  </si>
-  <si>
-    <t>leg_2_r</t>
-  </si>
-  <si>
-    <t>leg_3_r</t>
-  </si>
-  <si>
-    <t>R_Leg_1</t>
-  </si>
-  <si>
-    <t>R_Leg_2</t>
-  </si>
-  <si>
-    <t>R_Leg_3</t>
-  </si>
-  <si>
-    <t>Left Leg 2</t>
-  </si>
-  <si>
-    <t>Left Leg 3</t>
-  </si>
-  <si>
-    <t>Left Leg 1</t>
-  </si>
-  <si>
-    <t>leg_1_l</t>
-  </si>
-  <si>
-    <t>leg_2_l</t>
-  </si>
-  <si>
-    <t>leg_3_l</t>
-  </si>
-  <si>
-    <t>L_Leg_1</t>
-  </si>
-  <si>
-    <t>L_Leg_2</t>
-  </si>
-  <si>
-    <t>L_Leg_3</t>
-  </si>
-  <si>
-    <t>Shield 1</t>
-  </si>
-  <si>
-    <t>Shield 2</t>
-  </si>
-  <si>
-    <t>Shield 3</t>
-  </si>
-  <si>
-    <t>shield_1</t>
-  </si>
-  <si>
-    <t>shield_2</t>
-  </si>
-  <si>
-    <t>shield_3</t>
-  </si>
-  <si>
-    <t>Shield</t>
-  </si>
-  <si>
-    <t>Shield_1</t>
-  </si>
-  <si>
-    <t>Shield_2</t>
-  </si>
-  <si>
-    <t>Shield_3</t>
-  </si>
-  <si>
-    <t>weapon_1_r</t>
-  </si>
-  <si>
-    <t>weapon_2_r</t>
-  </si>
-  <si>
-    <t>weapon_1_l</t>
-  </si>
-  <si>
-    <t>weapon_2_l</t>
-  </si>
-  <si>
-    <t>R_Gladius_1</t>
-  </si>
-  <si>
-    <t>L_Gladius_1</t>
-  </si>
-  <si>
-    <t>R_Pugio_1</t>
-  </si>
-  <si>
-    <t>L_Pugio_1</t>
-  </si>
-  <si>
-    <t>Right Gladius 1</t>
-  </si>
-  <si>
-    <t>Left Gladius 1</t>
-  </si>
-  <si>
-    <t>Right Pugio 1</t>
-  </si>
-  <si>
-    <t>Left Pugio 1</t>
   </si>
 </sst>
 </file>
@@ -514,8 +496,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{5BA81B61-FF4B-4070-AFDD-483010E0F5E2}" name="Table18" displayName="Table18" ref="B5:F38" tableType="xml" totalsRowShown="0" connectionId="4">
-  <autoFilter ref="B5:F38" xr:uid="{9C5E23C4-2A17-4A45-9E0D-FA782667747E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{5BA81B61-FF4B-4070-AFDD-483010E0F5E2}" name="Table18" displayName="Table18" ref="B5:F36" tableType="xml" totalsRowShown="0" connectionId="4">
+  <autoFilter ref="B5:F36" xr:uid="{9C5E23C4-2A17-4A45-9E0D-FA782667747E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{20C3BA91-A104-45DF-8336-8663BB83979E}" uniqueName="Name" name="Name">
       <xmlColumnPr mapId="4" xpath="/ItemDataBase/Item/Name" xmlDataType="string"/>
@@ -836,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D766CA4A-594E-4340-8F54-93E0D16A5559}">
   <dimension ref="A5:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,10 +857,10 @@
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -887,15 +869,15 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -904,7 +886,7 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="Q7" t="s">
         <v>0</v>
@@ -924,10 +906,10 @@
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -936,7 +918,7 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -946,10 +928,10 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -958,15 +940,15 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
@@ -975,15 +957,15 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -992,15 +974,15 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -1009,15 +991,15 @@
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
@@ -1026,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1038,10 +1020,10 @@
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
         <v>27</v>
@@ -1050,128 +1032,128 @@
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1181,296 +1163,262 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" t="s">
         <v>81</v>
       </c>
-      <c r="C32" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" t="s">
-        <v>85</v>
-      </c>
       <c r="E32" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" t="s">
         <v>89</v>
       </c>
-      <c r="C34" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" t="s">
         <v>93</v>
-      </c>
-      <c r="E34" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" t="s">
         <v>90</v>
       </c>
-      <c r="C35" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" t="s">
         <v>94</v>
-      </c>
-      <c r="E35" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="F36" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" t="s">
-        <v>102</v>
-      </c>
-      <c r="E37" t="s">
-        <v>104</v>
-      </c>
-      <c r="F37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" t="s">
-        <v>100</v>
-      </c>
-      <c r="D38" t="s">
-        <v>103</v>
-      </c>
-      <c r="E38" t="s">
-        <v>104</v>
-      </c>
-      <c r="F38" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>